<commit_message>
not used files deleted
</commit_message>
<xml_diff>
--- a/Data/spring_data/peak_statistics/peak_statistics.xlsx
+++ b/Data/spring_data/peak_statistics/peak_statistics.xlsx
@@ -16,28 +16,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
-    <t>data duration</t>
-  </si>
-  <si>
-    <t>peak count</t>
-  </si>
-  <si>
-    <t>min width</t>
-  </si>
-  <si>
-    <t>1st quartile</t>
-  </si>
-  <si>
-    <t>median width</t>
-  </si>
-  <si>
-    <t>mean width</t>
-  </si>
-  <si>
-    <t>3rd quartile</t>
-  </si>
-  <si>
-    <t>max width</t>
+    <t>data_duration(days)</t>
+  </si>
+  <si>
+    <t>peak_count(-)</t>
+  </si>
+  <si>
+    <t>min_width(hours)</t>
+  </si>
+  <si>
+    <t>1st_quartile(hours)</t>
+  </si>
+  <si>
+    <t>median_width(hours)</t>
+  </si>
+  <si>
+    <t>mean_width(hours)</t>
+  </si>
+  <si>
+    <t>3rd_quartile(hours)</t>
+  </si>
+  <si>
+    <t>max_width(hours)</t>
   </si>
   <si>
     <t>Paliu_Fravi</t>
@@ -141,12 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,8 +476,8 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
-        <v>938.7218058217593</v>
+      <c r="B2">
+        <v>837</v>
       </c>
       <c r="C2">
         <v>21</v>
@@ -506,8 +505,8 @@
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
-        <v>236.1805555555555</v>
+      <c r="B3">
+        <v>179</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -536,7 +535,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -564,8 +563,8 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
-        <v>938.7225928587964</v>
+      <c r="B5">
+        <v>663</v>
       </c>
       <c r="C5">
         <v>23</v>
@@ -593,8 +592,8 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2">
-        <v>336.1458333333333</v>
+      <c r="B6">
+        <v>337</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -622,8 +621,8 @@
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2">
-        <v>336.2291666666667</v>
+      <c r="B7">
+        <v>337</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -651,8 +650,8 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2">
-        <v>216.9652777777778</v>
+      <c r="B8">
+        <v>202</v>
       </c>
       <c r="C8">
         <v>25</v>
@@ -680,8 +679,8 @@
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2">
-        <v>944.5825234143518</v>
+      <c r="B9">
+        <v>550</v>
       </c>
       <c r="C9">
         <v>19</v>
@@ -709,8 +708,8 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2">
-        <v>929.6737155439815</v>
+      <c r="B10">
+        <v>928</v>
       </c>
       <c r="C10">
         <v>71</v>
@@ -738,8 +737,8 @@
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2">
-        <v>555.4181828703704</v>
+      <c r="B11">
+        <v>500</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -767,8 +766,8 @@
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2">
-        <v>562.3117464699075</v>
+      <c r="B12">
+        <v>474</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -797,7 +796,7 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -825,8 +824,8 @@
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2">
-        <v>161.5833333333333</v>
+      <c r="B14">
+        <v>163</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -854,8 +853,8 @@
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2">
-        <v>156.5277777777778</v>
+      <c r="B15">
+        <v>158</v>
       </c>
       <c r="C15">
         <v>148</v>
@@ -883,8 +882,8 @@
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2">
-        <v>809.4003359143519</v>
+      <c r="B16">
+        <v>714</v>
       </c>
       <c r="C16">
         <v>80</v>

</xml_diff>

<commit_message>
temperature plots and temperature correlation added. Peak finding adjusted: prominence = 10% of mean discharge
</commit_message>
<xml_diff>
--- a/Data/spring_data/peak_statistics/peak_statistics.xlsx
+++ b/Data/spring_data/peak_statistics/peak_statistics.xlsx
@@ -55,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,42 +436,47 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>data duration</t>
+          <t>data_duration(days)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>peak count</t>
+          <t>peak_count(-)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>min width</t>
+          <t>mean_width(hours)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>1st quartile</t>
+          <t>std_width(hours)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>median width</t>
+          <t>min_width(hours)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>mean width</t>
+          <t>25%_width(hours)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>3rd quartile</t>
+          <t>50%_width(hours)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>max width</t>
+          <t>75%_width(hours)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>max_width(hours)</t>
         </is>
       </c>
     </row>
@@ -482,29 +486,32 @@
           <t>Paliu_Fravi</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>938.7218058217593</v>
+      <c r="B2" t="n">
+        <v>837</v>
       </c>
       <c r="C2" t="n">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="D2" t="n">
-        <v>3.844117447327181</v>
+        <v>22.26763770144503</v>
       </c>
       <c r="E2" t="n">
-        <v>6.379660926856014</v>
+        <v>27.25222656195201</v>
       </c>
       <c r="F2" t="n">
-        <v>8.755027487861298</v>
+        <v>4.435083017277611</v>
       </c>
       <c r="G2" t="n">
-        <v>20.57239771370926</v>
+        <v>8.546983716627034</v>
       </c>
       <c r="H2" t="n">
-        <v>17.7274514963734</v>
+        <v>12.11824252030929</v>
       </c>
       <c r="I2" t="n">
-        <v>120.4840153308716</v>
+        <v>21.44251670870872</v>
+      </c>
+      <c r="J2" t="n">
+        <v>141.1663359920239</v>
       </c>
     </row>
     <row r="3">
@@ -513,29 +520,32 @@
           <t>Salums_Friedrich</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>236.1805555555555</v>
+      <c r="B3" t="n">
+        <v>179</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>250.136556456608</v>
+        <v>134.3695290542638</v>
       </c>
       <c r="E3" t="n">
-        <v>250.136556456608</v>
+        <v>229.285170654976</v>
       </c>
       <c r="F3" t="n">
-        <v>250.136556456608</v>
+        <v>4.284756552016188</v>
       </c>
       <c r="G3" t="n">
-        <v>250.136556456608</v>
+        <v>6.375540697882707</v>
       </c>
       <c r="H3" t="n">
-        <v>250.136556456608</v>
+        <v>59.51568468468467</v>
       </c>
       <c r="I3" t="n">
-        <v>250.136556456608</v>
+        <v>60.04848668542981</v>
+      </c>
+      <c r="J3" t="n">
+        <v>541.6231766513058</v>
       </c>
     </row>
     <row r="4">
@@ -545,7 +555,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -568,6 +578,9 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -575,29 +588,32 @@
           <t>Leo_Friedrich</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>938.7225928587964</v>
+      <c r="B5" t="n">
+        <v>663</v>
       </c>
       <c r="C5" t="n">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="D5" t="n">
-        <v>1.53103025482369</v>
+        <v>6.555561813186176</v>
       </c>
       <c r="E5" t="n">
-        <v>2.642135176153357</v>
+        <v>24.4427667069091</v>
       </c>
       <c r="F5" t="n">
-        <v>3.645436625042385</v>
+        <v>0.2089729666471044</v>
       </c>
       <c r="G5" t="n">
-        <v>5.079260033263737</v>
+        <v>1.912510883512005</v>
       </c>
       <c r="H5" t="n">
-        <v>5.067949691882268</v>
+        <v>3.066037726782679</v>
       </c>
       <c r="I5" t="n">
-        <v>16.74308864931713</v>
+        <v>5.007662966679982</v>
+      </c>
+      <c r="J5" t="n">
+        <v>296.7230921080132</v>
       </c>
     </row>
     <row r="6">
@@ -606,29 +622,32 @@
           <t>Acqua_d'Balz_1</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>336.1458333333333</v>
+      <c r="B6" t="n">
+        <v>337</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D6" t="n">
-        <v>4.657852085766263</v>
+        <v>7.514852716775325</v>
       </c>
       <c r="E6" t="n">
-        <v>5.139973431128714</v>
+        <v>3.775813866971633</v>
       </c>
       <c r="F6" t="n">
-        <v>5.622094776491167</v>
+        <v>2.216579650084168</v>
       </c>
       <c r="G6" t="n">
-        <v>5.622094776491167</v>
+        <v>5.206373682363846</v>
       </c>
       <c r="H6" t="n">
-        <v>6.10421612185362</v>
+        <v>6.615741134061864</v>
       </c>
       <c r="I6" t="n">
-        <v>6.586337467216071</v>
+        <v>8.554663762121891</v>
+      </c>
+      <c r="J6" t="n">
+        <v>14.41948250415153</v>
       </c>
     </row>
     <row r="7">
@@ -637,29 +656,32 @@
           <t>Acqua_d'Balz_2</t>
         </is>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>336.2291666666667</v>
+      <c r="B7" t="n">
+        <v>337</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
-        <v>3.836402895420906</v>
+        <v>10.06178672462033</v>
       </c>
       <c r="E7" t="n">
-        <v>3.924753958102974</v>
+        <v>3.519286764977762</v>
       </c>
       <c r="F7" t="n">
-        <v>3.963254665288696</v>
+        <v>6.027402314650681</v>
       </c>
       <c r="G7" t="n">
-        <v>4.809408906688113</v>
+        <v>6.859573656117573</v>
       </c>
       <c r="H7" t="n">
-        <v>4.658995675267124</v>
+        <v>10.42345032769954</v>
       </c>
       <c r="I7" t="n">
-        <v>7.663637339360866</v>
+        <v>13.13167938931299</v>
+      </c>
+      <c r="J7" t="n">
+        <v>15.20838133891957</v>
       </c>
     </row>
     <row r="8">
@@ -668,29 +690,32 @@
           <t>Rossmoos</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>216.9652777777778</v>
+      <c r="B8" t="n">
+        <v>202</v>
       </c>
       <c r="C8" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D8" t="n">
-        <v>1.499310189595053</v>
+        <v>16.05063676518764</v>
       </c>
       <c r="E8" t="n">
-        <v>4.661623687342512</v>
+        <v>10.99396182937113</v>
       </c>
       <c r="F8" t="n">
-        <v>6.364924372652422</v>
+        <v>4.718047203911373</v>
       </c>
       <c r="G8" t="n">
-        <v>9.19572151899817</v>
+        <v>8.168644588095777</v>
       </c>
       <c r="H8" t="n">
-        <v>9.866505662589452</v>
+        <v>9.657039447704665</v>
       </c>
       <c r="I8" t="n">
-        <v>31.31562688211125</v>
+        <v>24.26244986044385</v>
+      </c>
+      <c r="J8" t="n">
+        <v>44.30537524634929</v>
       </c>
     </row>
     <row r="9">
@@ -699,29 +724,32 @@
           <t>Muesli</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>944.5825234143518</v>
+      <c r="B9" t="n">
+        <v>550</v>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6164757046601153</v>
+        <v>62.78907777518192</v>
       </c>
       <c r="E9" t="n">
-        <v>4.253851349918852</v>
+        <v>82.64458077130308</v>
       </c>
       <c r="F9" t="n">
-        <v>7.782498194109576</v>
+        <v>6.000210357707692</v>
       </c>
       <c r="G9" t="n">
-        <v>27.40619301696496</v>
+        <v>7.227354385528452</v>
       </c>
       <c r="H9" t="n">
-        <v>27.95049906576814</v>
+        <v>21.80692789610693</v>
       </c>
       <c r="I9" t="n">
-        <v>137.0977049288453</v>
+        <v>63.07202819440208</v>
+      </c>
+      <c r="J9" t="n">
+        <v>275.0706671806336</v>
       </c>
     </row>
     <row r="10">
@@ -730,29 +758,32 @@
           <t>Ulrika</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>929.6737155439815</v>
+      <c r="B10" t="n">
+        <v>928</v>
       </c>
       <c r="C10" t="n">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D10" t="n">
-        <v>0.284202989655023</v>
+        <v>29.63830998381162</v>
       </c>
       <c r="E10" t="n">
-        <v>5.992913005757146</v>
+        <v>21.15054197344147</v>
       </c>
       <c r="F10" t="n">
-        <v>14.19229743575852</v>
+        <v>1.423057632346172</v>
       </c>
       <c r="G10" t="n">
-        <v>17.43556527153404</v>
+        <v>16.30823221213249</v>
       </c>
       <c r="H10" t="n">
-        <v>26.88945888312082</v>
+        <v>23.14186141455939</v>
       </c>
       <c r="I10" t="n">
-        <v>58.87581010853901</v>
+        <v>38.3533105397395</v>
+      </c>
+      <c r="J10" t="n">
+        <v>106.1223488367574</v>
       </c>
     </row>
     <row r="11">
@@ -761,29 +792,32 @@
           <t>Chalta_Wasser</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>555.4181828703704</v>
+      <c r="B11" t="n">
+        <v>500</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>10.30637106705399</v>
+        <v>104.4137507953125</v>
       </c>
       <c r="E11" t="n">
-        <v>66.46957091503162</v>
+        <v>150.0506800357148</v>
       </c>
       <c r="F11" t="n">
-        <v>184.1452682953792</v>
+        <v>8.024916829093126</v>
       </c>
       <c r="G11" t="n">
-        <v>169.7060452850928</v>
+        <v>15.89198091324797</v>
       </c>
       <c r="H11" t="n">
-        <v>287.3817426654404</v>
+        <v>19.73415384615364</v>
       </c>
       <c r="I11" t="n">
-        <v>300.227273482559</v>
+        <v>105.8369444444445</v>
+      </c>
+      <c r="J11" t="n">
+        <v>413.0605028284102</v>
       </c>
     </row>
     <row r="12">
@@ -792,29 +826,32 @@
           <t>Grapp_rechts</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>562.3117464699075</v>
+      <c r="B12" t="n">
+        <v>474</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D12" t="n">
-        <v>9.007462353948359</v>
+        <v>34.02603493823661</v>
       </c>
       <c r="E12" t="n">
-        <v>9.876004976587865</v>
+        <v>33.08371545916909</v>
       </c>
       <c r="F12" t="n">
-        <v>15.62635969246185</v>
+        <v>3.579182735382346</v>
       </c>
       <c r="G12" t="n">
-        <v>24.17521794766013</v>
+        <v>14.34594828159243</v>
       </c>
       <c r="H12" t="n">
-        <v>31.71163192698732</v>
+        <v>26.45773504273511</v>
       </c>
       <c r="I12" t="n">
-        <v>68.51502664143845</v>
+        <v>41.7540026642906</v>
+      </c>
+      <c r="J12" t="n">
+        <v>168.7259467589109</v>
       </c>
     </row>
     <row r="13">
@@ -824,28 +861,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>34.24137495094337</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>13.19135388762352</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>24.91367916397326</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>29.57752705745832</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>34.24137495094337</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>38.90522284442844</v>
+      </c>
+      <c r="J13" t="n">
+        <v>43.56907073791349</v>
       </c>
     </row>
     <row r="14">
@@ -854,29 +894,30 @@
           <t>Prada_bella_sura</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>161.5833333333333</v>
+      <c r="B14" t="n">
+        <v>163</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>11.84962768755213</v>
-      </c>
-      <c r="E14" t="n">
-        <v>11.84962768755213</v>
-      </c>
+        <v>207.0200626522799</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>11.84962768755213</v>
+        <v>207.0200626522799</v>
       </c>
       <c r="G14" t="n">
-        <v>11.84962768755213</v>
+        <v>207.0200626522799</v>
       </c>
       <c r="H14" t="n">
-        <v>11.84962768755213</v>
+        <v>207.0200626522799</v>
       </c>
       <c r="I14" t="n">
-        <v>11.84962768755213</v>
+        <v>207.0200626522799</v>
+      </c>
+      <c r="J14" t="n">
+        <v>207.0200626522799</v>
       </c>
     </row>
     <row r="15">
@@ -885,29 +926,32 @@
           <t>Sarsura</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n">
-        <v>156.5277777777778</v>
+      <c r="B15" t="n">
+        <v>158</v>
       </c>
       <c r="C15" t="n">
-        <v>182</v>
+        <v>51</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1949482433448793</v>
+        <v>7.288532781307501</v>
       </c>
       <c r="E15" t="n">
-        <v>2.376152287862072</v>
+        <v>6.854258397270772</v>
       </c>
       <c r="F15" t="n">
-        <v>3.365961029661548</v>
+        <v>3.445716627738329</v>
       </c>
       <c r="G15" t="n">
-        <v>3.348168637336968</v>
+        <v>5.141625446740932</v>
       </c>
       <c r="H15" t="n">
-        <v>3.893662310368609</v>
+        <v>5.550719378836948</v>
       </c>
       <c r="I15" t="n">
-        <v>38.93705242120886</v>
+        <v>6.042061056025159</v>
+      </c>
+      <c r="J15" t="n">
+        <v>38.83186405252345</v>
       </c>
     </row>
     <row r="16">
@@ -916,29 +960,32 @@
           <t>Nidfuren</t>
         </is>
       </c>
-      <c r="B16" s="2" t="n">
-        <v>809.4003359143519</v>
+      <c r="B16" t="n">
+        <v>714</v>
       </c>
       <c r="C16" t="n">
-        <v>87</v>
+        <v>8</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2936328989439062</v>
+        <v>272.7212185548817</v>
       </c>
       <c r="E16" t="n">
-        <v>1.358179230155474</v>
+        <v>362.3565535276682</v>
       </c>
       <c r="F16" t="n">
-        <v>2.69072871889075</v>
+        <v>23.54000113646543</v>
       </c>
       <c r="G16" t="n">
-        <v>16.39435119069291</v>
+        <v>66.80345166302459</v>
       </c>
       <c r="H16" t="n">
-        <v>5.25819927100365</v>
+        <v>123.5790238833213</v>
       </c>
       <c r="I16" t="n">
-        <v>561.4546989265724</v>
+        <v>279.357899497555</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1094.592280242032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>